<commit_message>
edited for better layout
</commit_message>
<xml_diff>
--- a/Risikoanalyse.xlsx
+++ b/Risikoanalyse.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\EIT\FS19\pro2E\Team 5\P2Pflichtenheft\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BFE1ACC-B805-4505-BDB6-C83521079476}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94205051-8888-48A0-B2C1-D4C030EAEE9B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{47388EFE-A197-4ACA-8E67-E07DAE3FFCDF}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="108">
   <si>
     <t>Risiko</t>
   </si>
@@ -334,6 +334,30 @@
   </si>
   <si>
     <t>PL</t>
+  </si>
+  <si>
+    <t>Budgetüberschreitung</t>
+  </si>
+  <si>
+    <t>Mässig (1)</t>
+  </si>
+  <si>
+    <t>(fast) sicher
+&gt; 70%</t>
+  </si>
+  <si>
+    <t>Halb-halb 
+30% - 70%</t>
+  </si>
+  <si>
+    <t>Kaum 
+&lt; 30%</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt; 10% </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &gt; 25%</t>
   </si>
 </sst>
 </file>
@@ -435,7 +459,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -731,64 +755,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -806,54 +794,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -909,6 +849,128 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3289,789 +3351,887 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10FD6569-5768-494D-BE17-E5B41FC65FC6}">
-  <dimension ref="C3:R26"/>
+  <dimension ref="A1:P24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="3.44140625" customWidth="1"/>
-    <col min="4" max="4" width="17.21875" customWidth="1"/>
-    <col min="5" max="6" width="26.21875" customWidth="1"/>
-    <col min="7" max="9" width="6.44140625" customWidth="1"/>
-    <col min="10" max="11" width="26.21875" customWidth="1"/>
-    <col min="12" max="14" width="6.44140625" customWidth="1"/>
-    <col min="15" max="15" width="6.21875" customWidth="1"/>
-    <col min="16" max="16" width="9" customWidth="1"/>
-    <col min="17" max="17" width="3.77734375" customWidth="1"/>
-    <col min="18" max="18" width="43.44140625" customWidth="1"/>
+    <col min="1" max="1" width="3.44140625" customWidth="1"/>
+    <col min="2" max="2" width="17.21875" customWidth="1"/>
+    <col min="3" max="4" width="24.44140625" customWidth="1"/>
+    <col min="5" max="7" width="3.44140625" customWidth="1"/>
+    <col min="8" max="9" width="24.44140625" customWidth="1"/>
+    <col min="10" max="12" width="3.44140625" customWidth="1"/>
+    <col min="13" max="13" width="6.21875" customWidth="1"/>
+    <col min="14" max="14" width="9" customWidth="1"/>
+    <col min="15" max="15" width="3.77734375" customWidth="1"/>
+    <col min="16" max="16" width="43.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C3" s="44" t="s">
+    <row r="1" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44" t="s">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="K3" s="44"/>
-      <c r="L3" s="44"/>
-      <c r="M3" s="44"/>
-      <c r="N3" s="44"/>
-      <c r="O3" s="44"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
     </row>
-    <row r="4" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="C4" s="45" t="s">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="45" t="s">
+      <c r="B2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="45" t="s">
+      <c r="C2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="45" t="s">
+      <c r="D2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="46" t="s">
+      <c r="E2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="46" t="s">
+      <c r="F2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="46" t="s">
+      <c r="G2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="45" t="s">
+      <c r="H2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="K4" s="45" t="s">
+      <c r="I2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="46" t="s">
+      <c r="J2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="M4" s="46" t="s">
+      <c r="K2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="N4" s="46" t="s">
+      <c r="L2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="O4" s="46" t="s">
+      <c r="M2" s="9" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="5" spans="3:15" s="1" customFormat="1" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="47" t="s">
+    <row r="3" spans="1:13" s="1" customFormat="1" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="48" t="s">
+      <c r="B3" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="48" t="s">
+      <c r="C3" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="48" t="s">
+      <c r="D3" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G5" s="49">
+      <c r="E3" s="12">
         <v>3</v>
       </c>
-      <c r="H5" s="49">
+      <c r="F3" s="12">
         <v>2</v>
       </c>
-      <c r="I5" s="50">
+      <c r="G3" s="13">
         <v>6</v>
       </c>
-      <c r="J5" s="48" t="s">
+      <c r="H3" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="K5" s="48" t="s">
+      <c r="I3" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="L5" s="49">
+      <c r="J3" s="12">
         <v>3</v>
       </c>
-      <c r="M5" s="49">
+      <c r="K3" s="12">
         <v>1</v>
       </c>
-      <c r="N5" s="51">
+      <c r="L3" s="14">
         <v>3</v>
       </c>
-      <c r="O5" s="49" t="s">
+      <c r="M3" s="12" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="3:15" s="1" customFormat="1" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="47" t="s">
+    <row r="4" spans="1:13" s="1" customFormat="1" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="48" t="s">
+      <c r="B4" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="48" t="s">
+      <c r="C4" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="48" t="s">
+      <c r="D4" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="G6" s="49">
+      <c r="E4" s="12">
         <v>3</v>
       </c>
-      <c r="H6" s="49">
+      <c r="F4" s="12">
         <v>1</v>
       </c>
-      <c r="I6" s="51">
+      <c r="G4" s="14">
         <v>3</v>
       </c>
-      <c r="J6" s="48" t="s">
+      <c r="H4" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="K6" s="48" t="s">
+      <c r="I4" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="L6" s="49">
+      <c r="J4" s="12">
         <v>1</v>
       </c>
-      <c r="M6" s="49">
+      <c r="K4" s="12">
         <v>1</v>
       </c>
-      <c r="N6" s="52">
+      <c r="L4" s="15">
         <v>1</v>
       </c>
-      <c r="O6" s="49" t="s">
+      <c r="M4" s="12" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="3:15" s="1" customFormat="1" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="47" t="s">
+    <row r="5" spans="1:13" s="1" customFormat="1" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="48" t="s">
+      <c r="B5" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="48" t="s">
+      <c r="C5" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="48" t="s">
+      <c r="D5" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="G7" s="49">
+      <c r="E5" s="12">
         <v>3</v>
       </c>
-      <c r="H7" s="49">
+      <c r="F5" s="12">
         <v>1</v>
       </c>
-      <c r="I7" s="51">
+      <c r="G5" s="14">
         <v>3</v>
       </c>
-      <c r="J7" s="48" t="s">
+      <c r="H5" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="K7" s="48" t="s">
+      <c r="I5" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="L7" s="49">
+      <c r="J5" s="12">
         <v>1</v>
       </c>
-      <c r="M7" s="49">
+      <c r="K5" s="12">
         <v>1</v>
       </c>
-      <c r="N7" s="52">
+      <c r="L5" s="15">
         <v>1</v>
       </c>
-      <c r="O7" s="49" t="s">
+      <c r="M5" s="12" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="3:15" s="1" customFormat="1" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="47" t="s">
+    <row r="6" spans="1:13" s="1" customFormat="1" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="48" t="s">
+      <c r="B6" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="E8" s="48" t="s">
+      <c r="C6" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="48" t="s">
+      <c r="D6" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="G8" s="49">
+      <c r="E6" s="12">
         <v>3</v>
       </c>
-      <c r="H8" s="49">
+      <c r="F6" s="12">
         <v>1</v>
       </c>
-      <c r="I8" s="51">
+      <c r="G6" s="14">
         <v>3</v>
       </c>
-      <c r="J8" s="48" t="s">
+      <c r="H6" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="K8" s="48" t="s">
+      <c r="I6" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="L8" s="49">
+      <c r="J6" s="12">
         <v>1</v>
       </c>
-      <c r="M8" s="49">
+      <c r="K6" s="12">
         <v>1</v>
       </c>
-      <c r="N8" s="52">
+      <c r="L6" s="15">
         <v>1</v>
       </c>
-      <c r="O8" s="49" t="s">
+      <c r="M6" s="12" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="3:15" s="1" customFormat="1" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="47" t="s">
+    <row r="7" spans="1:13" s="1" customFormat="1" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="48" t="s">
+      <c r="B7" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="E9" s="48" t="s">
+      <c r="C7" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="48" t="s">
+      <c r="D7" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="G9" s="49">
+      <c r="E7" s="12">
         <v>2</v>
       </c>
-      <c r="H9" s="49">
+      <c r="F7" s="12">
         <v>2</v>
       </c>
-      <c r="I9" s="51">
+      <c r="G7" s="14">
         <v>4</v>
       </c>
-      <c r="J9" s="48" t="s">
+      <c r="H7" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="K9" s="48" t="s">
+      <c r="I7" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="L9" s="49">
+      <c r="J7" s="12">
         <v>2</v>
       </c>
-      <c r="M9" s="49">
+      <c r="K7" s="12">
         <v>1</v>
       </c>
-      <c r="N9" s="53">
+      <c r="L7" s="16">
         <v>2</v>
       </c>
-      <c r="O9" s="49" t="s">
+      <c r="M7" s="12" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="3:15" s="1" customFormat="1" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="47" t="s">
+    <row r="8" spans="1:13" s="1" customFormat="1" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="48" t="s">
+      <c r="B8" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="E10" s="48" t="s">
+      <c r="C8" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="F10" s="48" t="s">
+      <c r="D8" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="G10" s="49">
+      <c r="E8" s="12">
         <v>3</v>
       </c>
-      <c r="H10" s="49">
+      <c r="F8" s="12">
         <v>2</v>
       </c>
-      <c r="I10" s="50">
+      <c r="G8" s="13">
         <v>6</v>
       </c>
-      <c r="J10" s="48" t="s">
+      <c r="H8" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="K10" s="48" t="s">
+      <c r="I8" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="L10" s="49">
+      <c r="J8" s="12">
         <v>1</v>
       </c>
-      <c r="M10" s="49">
+      <c r="K8" s="12">
         <v>1</v>
       </c>
-      <c r="N10" s="52">
+      <c r="L8" s="15">
         <v>1</v>
       </c>
-      <c r="O10" s="49" t="s">
+      <c r="M8" s="12" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="3:15" s="1" customFormat="1" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="47" t="s">
+    <row r="9" spans="1:13" s="1" customFormat="1" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="48" t="s">
+      <c r="B9" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="E11" s="48" t="s">
+      <c r="C9" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="F11" s="48" t="s">
+      <c r="D9" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="G11" s="49">
+      <c r="E9" s="12">
         <v>2</v>
       </c>
-      <c r="H11" s="49">
+      <c r="F9" s="12">
         <v>2</v>
       </c>
-      <c r="I11" s="51">
+      <c r="G9" s="14">
         <v>4</v>
       </c>
-      <c r="J11" s="48" t="s">
+      <c r="H9" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="K11" s="48" t="s">
+      <c r="I9" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="L11" s="49">
+      <c r="J9" s="12">
         <v>1</v>
       </c>
-      <c r="M11" s="49">
+      <c r="K9" s="12">
         <v>1</v>
       </c>
-      <c r="N11" s="52">
+      <c r="L9" s="15">
         <v>1</v>
       </c>
-      <c r="O11" s="49" t="s">
+      <c r="M9" s="12" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="3:15" s="1" customFormat="1" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="47" t="s">
+    <row r="10" spans="1:13" s="1" customFormat="1" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="48" t="s">
+      <c r="B10" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="E12" s="48" t="s">
+      <c r="C10" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="F12" s="48" t="s">
+      <c r="D10" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="G12" s="49">
+      <c r="E10" s="12">
         <v>2</v>
       </c>
-      <c r="H12" s="49">
+      <c r="F10" s="12">
         <v>2</v>
       </c>
-      <c r="I12" s="51">
+      <c r="G10" s="14">
         <v>4</v>
       </c>
-      <c r="J12" s="48" t="s">
+      <c r="H10" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="K12" s="48" t="s">
+      <c r="I10" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="L12" s="49">
+      <c r="J10" s="12">
         <v>2</v>
       </c>
-      <c r="M12" s="49">
+      <c r="K10" s="12">
         <v>1</v>
       </c>
-      <c r="N12" s="53">
+      <c r="L10" s="16">
         <v>2</v>
       </c>
-      <c r="O12" s="49" t="s">
+      <c r="M10" s="12" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="13" spans="3:15" s="1" customFormat="1" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="47" t="s">
+    <row r="11" spans="1:13" s="1" customFormat="1" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="48" t="s">
+      <c r="B11" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="E13" s="48" t="s">
+      <c r="C11" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="F13" s="48" t="s">
+      <c r="D11" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="G13" s="49">
+      <c r="E11" s="12">
         <v>1</v>
       </c>
-      <c r="H13" s="49">
+      <c r="F11" s="12">
         <v>3</v>
       </c>
-      <c r="I13" s="51">
+      <c r="G11" s="14">
         <v>3</v>
       </c>
-      <c r="J13" s="48" t="s">
+      <c r="H11" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="K13" s="48" t="s">
+      <c r="I11" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="L13" s="49">
+      <c r="J11" s="12">
         <v>1</v>
       </c>
-      <c r="M13" s="49">
+      <c r="K11" s="12">
         <v>1</v>
       </c>
-      <c r="N13" s="52">
+      <c r="L11" s="15">
         <v>1</v>
       </c>
-      <c r="O13" s="49" t="s">
+      <c r="M11" s="12" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="3:15" s="1" customFormat="1" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="47" t="s">
+    <row r="12" spans="1:13" s="1" customFormat="1" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="D14" s="48" t="s">
+      <c r="B12" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="E14" s="48" t="s">
+      <c r="C12" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="F14" s="48" t="s">
+      <c r="D12" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="G14" s="49">
+      <c r="E12" s="12">
         <v>3</v>
       </c>
-      <c r="H14" s="49">
+      <c r="F12" s="12">
         <v>2</v>
       </c>
-      <c r="I14" s="50">
+      <c r="G12" s="13">
         <v>6</v>
       </c>
-      <c r="J14" s="48" t="s">
+      <c r="H12" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="K14" s="48" t="s">
+      <c r="I12" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="L14" s="49">
+      <c r="J12" s="12">
         <v>2</v>
       </c>
-      <c r="M14" s="49">
+      <c r="K12" s="12">
         <v>1</v>
       </c>
-      <c r="N14" s="53">
+      <c r="L12" s="16">
         <v>2</v>
       </c>
-      <c r="O14" s="49" t="s">
+      <c r="M12" s="12" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="3:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="54" t="s">
+    <row r="13" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="55"/>
-      <c r="E15" s="55"/>
-      <c r="F15" s="55"/>
-      <c r="G15" s="56"/>
-      <c r="H15" s="56"/>
-      <c r="I15" s="56"/>
-      <c r="J15" s="55"/>
-      <c r="K15" s="55"/>
-      <c r="L15" s="56"/>
-      <c r="M15" s="56"/>
-      <c r="N15" s="56"/>
-      <c r="O15" s="57"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="19"/>
+      <c r="M13" s="20"/>
     </row>
-    <row r="16" spans="3:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="58" t="s">
+    <row r="14" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="48"/>
-      <c r="E16" s="48"/>
-      <c r="F16" s="48"/>
-      <c r="G16" s="49"/>
-      <c r="H16" s="49"/>
-      <c r="I16" s="49"/>
-      <c r="J16" s="48"/>
-      <c r="K16" s="48"/>
-      <c r="L16" s="49"/>
-      <c r="M16" s="49"/>
-      <c r="N16" s="49"/>
-      <c r="O16" s="59"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="22"/>
     </row>
-    <row r="17" spans="3:18" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C17" s="60" t="s">
+    <row r="15" spans="1:13" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="D17" s="61"/>
-      <c r="E17" s="61"/>
-      <c r="F17" s="61"/>
-      <c r="G17" s="62"/>
-      <c r="H17" s="62"/>
-      <c r="I17" s="62"/>
-      <c r="J17" s="61"/>
-      <c r="K17" s="61"/>
-      <c r="L17" s="62"/>
-      <c r="M17" s="62"/>
-      <c r="N17" s="62"/>
-      <c r="O17" s="63"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="25"/>
+      <c r="K15" s="25"/>
+      <c r="L15" s="25"/>
+      <c r="M15" s="26"/>
     </row>
-    <row r="18" spans="3:18" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="19" spans="3:18" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="20" spans="3:18" s="1" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="Q20" s="35" t="s">
+    <row r="16" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="15:16" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="18" spans="15:16" s="1" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="O18" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="R20" s="36"/>
+      <c r="P18" s="29"/>
     </row>
-    <row r="21" spans="3:18" x14ac:dyDescent="0.3">
-      <c r="Q21" s="21" t="s">
+    <row r="19" spans="15:16" x14ac:dyDescent="0.3">
+      <c r="O19" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="R21" s="22" t="s">
+      <c r="P19" s="3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="3:18" x14ac:dyDescent="0.3">
-      <c r="Q22" s="23" t="s">
+    <row r="20" spans="15:16" x14ac:dyDescent="0.3">
+      <c r="O20" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="R22" s="24" t="s">
+      <c r="P20" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="3:18" x14ac:dyDescent="0.3">
-      <c r="Q23" s="23" t="s">
+    <row r="21" spans="15:16" x14ac:dyDescent="0.3">
+      <c r="O21" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="R23" s="24" t="s">
+      <c r="P21" s="5" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="3:18" x14ac:dyDescent="0.3">
-      <c r="Q24" s="23" t="s">
+    <row r="22" spans="15:16" x14ac:dyDescent="0.3">
+      <c r="O22" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="R24" s="24" t="s">
+      <c r="P22" s="5" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="3:18" x14ac:dyDescent="0.3">
-      <c r="Q25" s="23" t="s">
+    <row r="23" spans="15:16" x14ac:dyDescent="0.3">
+      <c r="O23" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="R25" s="24" t="s">
+      <c r="P23" s="5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="26" spans="3:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="Q26" s="25" t="s">
+    <row r="24" spans="15:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="O24" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="R26" s="26" t="s">
+      <c r="P24" s="7" t="s">
         <v>66</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="C3:I3"/>
-    <mergeCell ref="J3:O3"/>
-    <mergeCell ref="Q20:R20"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="H1:M1"/>
+    <mergeCell ref="O18:P18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFD7A736-9363-4CF6-BDAA-9052391D740B}">
-  <dimension ref="B2:K19"/>
+  <dimension ref="B2:P29"/>
   <sheetViews>
-    <sheetView topLeftCell="F15" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22:P29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.44140625" customWidth="1"/>
-    <col min="3" max="5" width="12.77734375" customWidth="1"/>
-    <col min="7" max="7" width="3.5546875" customWidth="1"/>
-    <col min="8" max="8" width="8.6640625" customWidth="1"/>
-    <col min="9" max="11" width="30.6640625" customWidth="1"/>
+    <col min="1" max="1" width="11.5546875" style="30"/>
+    <col min="2" max="2" width="14.44140625" style="30" customWidth="1"/>
+    <col min="3" max="5" width="12.77734375" style="30" customWidth="1"/>
+    <col min="6" max="6" width="11.5546875" style="30"/>
+    <col min="7" max="7" width="3.5546875" style="30" customWidth="1"/>
+    <col min="8" max="8" width="8.6640625" style="30" customWidth="1"/>
+    <col min="9" max="11" width="30.6640625" style="30" customWidth="1"/>
+    <col min="12" max="12" width="11.5546875" style="30"/>
+    <col min="13" max="13" width="20.6640625" style="30" customWidth="1"/>
+    <col min="14" max="16" width="15.109375" style="30" customWidth="1"/>
+    <col min="17" max="16384" width="11.5546875" style="30"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C2" s="37" t="s">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C2" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B3" s="3" t="s">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B3" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="34" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B4" s="7" t="s">
+    <row r="4" spans="2:11" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="B4" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="36" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B5" s="3" t="s">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="36" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C9" s="37" t="s">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C9" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="D9" s="37"/>
-      <c r="E9" s="37"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B10" s="9"/>
-      <c r="C10" s="4" t="s">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10" s="37"/>
+      <c r="C10" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="34" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B11" s="7" t="s">
+    <row r="11" spans="2:11" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="B11" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="12" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="2:11" ht="90" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="2:11" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G15" s="38" t="s">
         <v>96</v>
       </c>
-      <c r="H15" s="27" t="s">
+      <c r="H15" s="39" t="s">
         <v>85</v>
       </c>
-      <c r="I15" s="13">
+      <c r="I15" s="40">
         <v>3</v>
       </c>
-      <c r="J15" s="14">
+      <c r="J15" s="41">
         <v>6</v>
       </c>
-      <c r="K15" s="15">
+      <c r="K15" s="42">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="2:11" ht="90" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G16" s="39"/>
-      <c r="H16" s="11" t="s">
+    <row r="16" spans="2:11" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G16" s="43"/>
+      <c r="H16" s="44" t="s">
         <v>84</v>
       </c>
-      <c r="I16" s="16">
+      <c r="I16" s="45">
         <v>2</v>
       </c>
-      <c r="J16" s="10">
+      <c r="J16" s="46">
         <v>4</v>
       </c>
-      <c r="K16" s="17">
+      <c r="K16" s="47">
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="7:11" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G17" s="40"/>
-      <c r="H17" s="30" t="s">
+    <row r="17" spans="7:16" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G17" s="48"/>
+      <c r="H17" s="49" t="s">
         <v>83</v>
       </c>
-      <c r="I17" s="18">
+      <c r="I17" s="50">
         <v>1</v>
       </c>
-      <c r="J17" s="19">
+      <c r="J17" s="51">
         <v>2</v>
       </c>
-      <c r="K17" s="20">
+      <c r="K17" s="52">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="7:11" x14ac:dyDescent="0.3">
-      <c r="G18" s="32"/>
-      <c r="H18" s="31"/>
-      <c r="I18" s="29" t="s">
+    <row r="18" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="G18" s="53"/>
+      <c r="H18" s="54"/>
+      <c r="I18" s="55" t="s">
         <v>83</v>
       </c>
-      <c r="J18" s="12" t="s">
+      <c r="J18" s="56" t="s">
         <v>84</v>
       </c>
-      <c r="K18" s="28" t="s">
+      <c r="K18" s="57" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="7:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G19" s="33"/>
-      <c r="H19" s="34"/>
-      <c r="I19" s="41" t="s">
+    <row r="19" spans="7:16" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G19" s="58"/>
+      <c r="H19" s="59"/>
+      <c r="I19" s="60" t="s">
         <v>97</v>
       </c>
-      <c r="J19" s="42"/>
-      <c r="K19" s="43"/>
+      <c r="J19" s="61"/>
+      <c r="K19" s="62"/>
+    </row>
+    <row r="22" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="M22" s="63"/>
+      <c r="N22" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="O22" s="31"/>
+      <c r="P22" s="31"/>
+    </row>
+    <row r="23" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="M23" s="63" t="s">
+        <v>68</v>
+      </c>
+      <c r="N23" s="70" t="s">
+        <v>70</v>
+      </c>
+      <c r="O23" s="71" t="s">
+        <v>102</v>
+      </c>
+      <c r="P23" s="72" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="M24" s="63" t="s">
+        <v>101</v>
+      </c>
+      <c r="N24" s="64" t="s">
+        <v>106</v>
+      </c>
+      <c r="O24" s="64" t="s">
+        <v>76</v>
+      </c>
+      <c r="P24" s="64" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="25" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="M25" s="63" t="s">
+        <v>73</v>
+      </c>
+      <c r="N25" s="64" t="s">
+        <v>106</v>
+      </c>
+      <c r="O25" s="64" t="s">
+        <v>76</v>
+      </c>
+      <c r="P25" s="64" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="26" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="N26" s="68"/>
+      <c r="O26" s="68"/>
+      <c r="P26" s="68"/>
+    </row>
+    <row r="27" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="M27" s="65"/>
+      <c r="N27" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="O27" s="31"/>
+      <c r="P27" s="31"/>
+    </row>
+    <row r="28" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="M28" s="66"/>
+      <c r="N28" s="70" t="s">
+        <v>70</v>
+      </c>
+      <c r="O28" s="71" t="s">
+        <v>102</v>
+      </c>
+      <c r="P28" s="72" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29" spans="7:16" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M29" s="67" t="s">
+        <v>79</v>
+      </c>
+      <c r="N29" s="69" t="s">
+        <v>105</v>
+      </c>
+      <c r="O29" s="69" t="s">
+        <v>104</v>
+      </c>
+      <c r="P29" s="69" t="s">
+        <v>103</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="7">
+    <mergeCell ref="N27:P27"/>
+    <mergeCell ref="M27:M28"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="C9:E9"/>
     <mergeCell ref="G15:G17"/>
     <mergeCell ref="I19:K19"/>
+    <mergeCell ref="N22:P22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>